<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@b4be94c21c6e10df5d19499e641b0add9d1d4c87 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-family-role.xlsx
+++ b/StructureDefinition-family-role.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-13T20:57:31+00:00</t>
+    <t>2024-09-16T16:04:42+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Element</t>
+    <t>element:Group.content.extension</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@01aeeba9013e134e1db03c4302da92843ab5202b 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-family-role.xlsx
+++ b/StructureDefinition-family-role.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-16T16:04:42+00:00</t>
+    <t>2024-09-18T19:34:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Group.content.extension</t>
+    <t>element:Group.member.entity</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>